<commit_message>
agregado lectura de Usuarios para login
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41cd670604df91f8/UH/11vo Cuatri/Progra IV/Proyecto1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridia\source\repos\Medical App\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{9980535E-6F86-40F7-9764-805231CE4669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1D31F39-9687-43F2-AA3D-4581B0D25E6F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB8A347-E401-4DC4-81F7-FB85A0BE255F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
+    <workbookView xWindow="-41388" yWindow="-36" windowWidth="41496" windowHeight="16776" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Usuario</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>Rol</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>administrador</t>
   </si>
 </sst>
 </file>
@@ -184,11 +190,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -526,11 +532,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4CEB0A7-F569-444F-BECD-CF937D694833}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -547,10 +556,18 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2">
+        <v>123</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -601,40 +618,40 @@
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -850,52 +867,52 @@
       <c r="P1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -1459,7 +1476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0852A8F-B607-4A83-B14C-ED5F14713E4C}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
login funcionando. falta redireccionar a otras paginas dependiendo si es admin o medico
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridia\source\repos\Medical App\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB8A347-E401-4DC4-81F7-FB85A0BE255F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263605D9-C4A5-401A-86D4-110791262362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-41388" yWindow="-36" windowWidth="41496" windowHeight="16776" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
@@ -193,7 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -533,7 +533,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
agregada funcion de dar click para ver enfermedades del paciente
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridia\source\repos\Medical App\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA99D468-3335-4B30-93C3-C233DDE576CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2338FDF-9A53-4DB9-AF63-5FEC8C94D482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
     <sheet name="Sucursales" sheetId="4" r:id="rId2"/>
     <sheet name="Enfermedades" sheetId="6" r:id="rId3"/>
-    <sheet name="Medicamentos" sheetId="5" r:id="rId4"/>
-    <sheet name="Pacientes" sheetId="3" r:id="rId5"/>
+    <sheet name="Medicamentos" sheetId="8" r:id="rId4"/>
+    <sheet name="Pacientes" sheetId="7" r:id="rId5"/>
     <sheet name="Medicos" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -340,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -349,13 +349,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -960,21 +953,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2908B4BF-E48D-481B-94FC-583924661663}">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F1A546-74ED-4339-A07B-8B9763880824}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="5"/>
-    <col min="3" max="3" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="5"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1031,36 +1017,6 @@
       <c r="D4" s="3">
         <v>150</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1068,33 +1024,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52B00F8D-6F86-4C72-B8A1-FF2C95466990}">
-  <dimension ref="A1:R4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681C15B9-EC30-4BAF-91C3-5E6E8A5EFD20}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="5"/>
-    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="5" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="11" style="5" customWidth="1"/>
-    <col min="12" max="12" width="22.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="5"/>
+    <col min="1" max="1" width="2.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -1131,14 +1083,8 @@
       <c r="L1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1160,7 +1106,7 @@
       <c r="G2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="4">
         <v>32874</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -1175,14 +1121,8 @@
       <c r="L2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1204,7 +1144,7 @@
       <c r="G3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="4">
         <v>31213</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -1219,14 +1159,8 @@
       <c r="L3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1248,7 +1182,7 @@
       <c r="G4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="4">
         <v>34768</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -1273,24 +1207,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E48C19A-0310-4CEF-960B-0D22DFA9D7E7}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.75" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="5"/>
-    <col min="10" max="10" width="9.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="5"/>
+    <col min="1" max="1" width="2.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1350,7 +1282,7 @@
       <c r="G2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="4">
         <v>31079</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -1385,7 +1317,7 @@
       <c r="G3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="4">
         <v>28689</v>
       </c>
       <c r="I3" s="3" t="s">
@@ -1420,7 +1352,7 @@
       <c r="G4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="4">
         <v>33918</v>
       </c>
       <c r="I4" s="3" t="s">
@@ -1434,88 +1366,88 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
arreglo error con funcion bCitas
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridia\source\repos\Medical App\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CF3CB0-51F7-42D7-9CE9-FDABB06FB093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112783D6-CB1C-439A-8FE9-2E9EA7448A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-41388" yWindow="-36" windowWidth="41496" windowHeight="16776" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="89">
   <si>
     <t>Usuario</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>Ginecologia</t>
+  </si>
+  <si>
+    <t>medico</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,6 +375,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B0FDD3-0092-4C45-AB58-9DA5CB91D551}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,6 +749,20 @@
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="5">
+        <v>123</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aquí van los cambios de agregar, faltan en algunas variables
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridia\source\repos\Medical App\Medical App\Uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rivas\source\repos\Medical-App3\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112783D6-CB1C-439A-8FE9-2E9EA7448A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BD6482-35ED-4009-A6AB-D3892CA6FBA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41388" yWindow="-36" windowWidth="41496" windowHeight="16776" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
   <si>
     <t>Usuario</t>
   </si>
@@ -298,23 +298,20 @@
     <t>Especialidad</t>
   </si>
   <si>
-    <t>Medicina General</t>
-  </si>
-  <si>
-    <t>Cardiologia</t>
-  </si>
-  <si>
-    <t>Ginecologia</t>
-  </si>
-  <si>
     <t>medico</t>
+  </si>
+  <si>
+    <t>wasabi@gmail.com</t>
+  </si>
+  <si>
+    <t>guillermo@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -377,6 +374,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,19 +721,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B0FDD3-0092-4C45-AB58-9DA5CB91D551}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -737,36 +747,65 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="6">
         <v>123</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="5">
+        <v>85</v>
+      </c>
+      <c r="C3" s="7">
         <v>123</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="7">
+        <v>456</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="7">
+        <v>456</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -778,12 +817,12 @@
       <selection sqref="A1:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -797,7 +836,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -811,7 +850,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -825,7 +864,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -850,12 +889,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="56.25" customWidth="1"/>
+    <col min="2" max="2" width="56.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="20.399999999999999">
       <c r="A1" s="4" t="s">
         <v>82</v>
       </c>
@@ -866,7 +905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -877,7 +916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -888,7 +927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -912,12 +951,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -931,7 +970,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -945,7 +984,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -959,7 +998,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -986,22 +1025,22 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="2.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.8984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -1039,7 +1078,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1077,7 +1116,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1115,7 +1154,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1159,174 +1198,220 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5DCD55-2C2D-467A-B803-E34BF93AA1ED}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="2.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.3984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.796875" style="9"/>
+    <col min="4" max="4" width="16.8984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.796875" style="9"/>
+    <col min="7" max="7" width="9.3984375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.296875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="8.796875" style="9"/>
+    <col min="11" max="11" width="21.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.69921875" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.796875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row spans="1:11" outlineLevel="0" r="1">
+      <c r="A1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    </row>
+    <row spans="1:11" outlineLevel="0" r="2">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="10" t="s">
         <v>51</v>
       </c>
       <c r="H2" s="3">
         <v>31079</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    </row>
+    <row spans="1:11" outlineLevel="0" r="3">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="8">
         <v>123456789</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="10" t="s">
         <v>60</v>
       </c>
       <c r="H3" s="3">
         <v>28689</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
+    </row>
+    <row spans="1:11" outlineLevel="0" r="4">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="8">
         <v>987654321</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="10" t="s">
         <v>51</v>
       </c>
       <c r="H4" s="3">
         <v>33918</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>87</v>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="C5" s="10" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="F5" s="10" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="G5" s="10" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="H5" s="3">
+        <v>45120.5</v>
+      </c>
+      <c r="I5" s="10" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
+      </c>
+      <c r="J5" s="10" t="inlineStr">
+        <is>
+          <t>54125</t>
+        </is>
+      </c>
+      <c r="K5" s="10" t="inlineStr">
+        <is>
+          <t>ss</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Insertar en todos menos en Paciente porque otro compañero lo hizo
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rivas\source\repos\Medical-App3\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BD6482-35ED-4009-A6AB-D3892CA6FBA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FC29A0-B44E-4497-BCCD-9148E49546E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="3" activeTab="5" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="10" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
   <si>
     <t>Usuario</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Teléfono</t>
   </si>
   <si>
-    <t>Correo electrónico</t>
-  </si>
-  <si>
     <t>San José</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>Nombre de enfermedad</t>
-  </si>
-  <si>
     <t>Dengue</t>
   </si>
   <si>
@@ -305,6 +299,24 @@
   </si>
   <si>
     <t>guillermo@gmail.com</t>
+  </si>
+  <si>
+    <t>ss</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>ssss</t>
+  </si>
+  <si>
+    <t>Enfermedad</t>
+  </si>
+  <si>
+    <t>dsd</t>
+  </si>
+  <si>
+    <t>sds</t>
   </si>
 </sst>
 </file>
@@ -360,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -384,10 +396,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,13 +784,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C3" s="7">
         <v>123</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -780,7 +798,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" s="7">
         <v>456</v>
@@ -794,13 +812,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C5" s="7">
         <v>456</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -811,71 +829,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349371A3-B132-4D64-BA53-AC966C95A385}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.796875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -885,21 +918,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0852A8F-B607-4A83-B14C-ED5F14713E4C}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
     <col min="2" max="2" width="56.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.399999999999999">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -910,10 +945,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -921,10 +956,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -932,10 +967,21 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -945,10 +991,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F1A546-74ED-4339-A07B-8B9763880824}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
@@ -958,16 +1004,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -975,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2">
         <v>100</v>
@@ -989,10 +1035,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2">
         <v>200</v>
@@ -1003,13 +1049,27 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2">
         <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1042,28 +1102,28 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
@@ -1075,7 +1135,7 @@
         <v>14</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1083,37 +1143,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="E2" s="2">
         <v>123456789</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H2" s="3">
         <v>32874</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1121,37 +1181,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="H3" s="3">
         <v>31213</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1159,37 +1219,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2">
         <v>456789123</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4" s="3">
         <v>34768</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1198,220 +1258,167 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="2.3984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.796875" style="9"/>
-    <col min="4" max="4" width="16.8984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.796875" style="9"/>
-    <col min="7" max="7" width="9.3984375" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.296875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="12.59765625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="8.796875" style="9"/>
-    <col min="11" max="11" width="21.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.69921875" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.796875" style="9"/>
+    <col min="1" max="1" width="4.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.796875" style="10"/>
+    <col min="4" max="4" width="16.8984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.796875" style="10"/>
+    <col min="7" max="7" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.296875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="8.796875" style="10"/>
+    <col min="11" max="11" width="21.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.69921875" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.796875" style="10"/>
   </cols>
   <sheetData>
-    <row spans="1:11" outlineLevel="0" r="1">
-      <c r="A1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="I1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row spans="1:11" outlineLevel="0" r="2">
-      <c r="A2" s="10">
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>51</v>
+      <c r="F2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="H2" s="3">
         <v>31079</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="10" t="s">
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row spans="1:11" outlineLevel="0" r="3">
-      <c r="A3" s="10">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>49</v>
+      <c r="C3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="E3" s="8">
         <v>123456789</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>60</v>
+      <c r="F3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="H3" s="3">
         <v>28689</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="10" t="s">
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="C4" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row spans="1:11" outlineLevel="0" r="4">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>49</v>
+      <c r="D4" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="E4" s="8">
         <v>987654321</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>51</v>
+      <c r="F4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="H4" s="3">
         <v>33918</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="12" t="s">
         <v>79</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="5">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-      <c r="C5" s="10" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-      <c r="D5" s="10" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-      <c r="E5" s="10" t="inlineStr">
-        <is>
-          <t>12345</t>
-        </is>
-      </c>
-      <c r="F5" s="10" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-      <c r="G5" s="10" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-      <c r="H5" s="3">
-        <v>45120.5</v>
-      </c>
-      <c r="I5" s="10" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
-      </c>
-      <c r="J5" s="10" t="inlineStr">
-        <is>
-          <t>54125</t>
-        </is>
-      </c>
-      <c r="K5" s="10" t="inlineStr">
-        <is>
-          <t>ss</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios en las funciones. arreglando funciones de insertar. cierra el form de insertar, refresca la tabla, muestra mensaje de exito
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rivas\source\repos\Medical-App3\Medical App\Uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridia\source\repos\Medical App\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FC29A0-B44E-4497-BCCD-9148E49546E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B485BCB-36FB-4E9B-A9AC-01989D2DBCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="3" activeTab="5" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="10" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Medicamentos" sheetId="8" r:id="rId4"/>
     <sheet name="Pacientes" sheetId="7" r:id="rId5"/>
     <sheet name="Medicos" sheetId="9" r:id="rId6"/>
+    <sheet name="Expedientes" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="101">
   <si>
     <t>Usuario</t>
   </si>
@@ -283,9 +284,6 @@
     <t>roberto.m@example.com</t>
   </si>
   <si>
-    <t>IdPaciente</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -317,13 +315,43 @@
   </si>
   <si>
     <t>sds</t>
+  </si>
+  <si>
+    <t>Medicamentos</t>
+  </si>
+  <si>
+    <t>Indicaciones</t>
+  </si>
+  <si>
+    <t>fechaPrescripcion</t>
+  </si>
+  <si>
+    <t>especialidadMedico</t>
+  </si>
+  <si>
+    <t>fechaCita</t>
+  </si>
+  <si>
+    <t>fechaNacimiento</t>
+  </si>
+  <si>
+    <t>apellido2</t>
+  </si>
+  <si>
+    <t>apellido1</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>idPaciente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -397,11 +425,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -739,19 +762,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" rightToLeft="false">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -765,7 +788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -779,26 +802,26 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="7">
         <v>123</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>82</v>
+      </c>
+    </row>
+    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="7">
         <v>456</v>
@@ -807,18 +830,338 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="7">
         <v>456</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t>medico</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" s="9" t="inlineStr">
+        <is>
+          <t>medico</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="9">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="C8" s="9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" s="9" t="inlineStr">
+        <is>
+          <t>medico</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="9">
+        <v>1</v>
+      </c>
+      <c r="B9" s="9" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="C9" s="9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>medico</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="9">
+        <v>1</v>
+      </c>
+      <c r="B10" s="9" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="C10" s="9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" s="9" t="inlineStr">
+        <is>
+          <t>medico</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="9">
+        <v>1</v>
+      </c>
+      <c r="B11" s="9" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="C11" s="9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D11" s="9" t="inlineStr">
+        <is>
+          <t>medico</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="9">
+        <v>1</v>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>rrr</t>
+        </is>
+      </c>
+      <c r="C12" s="9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D12" s="9" t="inlineStr">
+        <is>
+          <t>medico</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="9">
+        <v>1</v>
+      </c>
+      <c r="B13" s="9" t="inlineStr">
+        <is>
+          <t>ffaf</t>
+        </is>
+      </c>
+      <c r="C13" s="9" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="D13" s="9" t="inlineStr">
+        <is>
+          <t>fafafa</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="14">
+      <c r="A14" s="9">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9" t="inlineStr">
+        <is>
+          <t>ffaf</t>
+        </is>
+      </c>
+      <c r="C14" s="9" t="inlineStr">
+        <is>
+          <t>fff</t>
+        </is>
+      </c>
+      <c r="D14" s="9" t="inlineStr">
+        <is>
+          <t>fafafa</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="15">
+      <c r="A15" s="9">
+        <v>41713</v>
+      </c>
+      <c r="B15" s="9" t="inlineStr">
+        <is>
+          <t>rdiazelx@gmail.com</t>
+        </is>
+      </c>
+      <c r="C15" s="9" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D15" s="9" t="inlineStr">
+        <is>
+          <t>medico</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="16">
+      <c r="A16" s="9">
+        <v>75928</v>
+      </c>
+      <c r="B16" s="9" t="inlineStr">
+        <is>
+          <t>rttt</t>
+        </is>
+      </c>
+      <c r="C16" s="9" t="inlineStr">
+        <is>
+          <t>tttt</t>
+        </is>
+      </c>
+      <c r="D16" s="9" t="inlineStr">
+        <is>
+          <t>ttt</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="17">
+      <c r="A17" s="9">
+        <v>16425</v>
+      </c>
+      <c r="B17" s="9" t="inlineStr">
+        <is>
+          <t>rdiazelx@gmail.com</t>
+        </is>
+      </c>
+      <c r="C17" s="9" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D17" s="9" t="inlineStr">
+        <is>
+          <t>administrador</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="18">
+      <c r="A18" s="9">
+        <v>54053</v>
+      </c>
+      <c r="B18" s="9" t="inlineStr">
+        <is>
+          <t>jack</t>
+        </is>
+      </c>
+      <c r="C18" s="9" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="D18" s="9" t="inlineStr">
+        <is>
+          <t>medico</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="19">
+      <c r="A19" s="9">
+        <v>79710</v>
+      </c>
+      <c r="B19" s="9" t="inlineStr">
+        <is>
+          <t>prueba</t>
+        </is>
+      </c>
+      <c r="C19" s="9" t="inlineStr">
+        <is>
+          <t>prueba</t>
+        </is>
+      </c>
+      <c r="D19" s="9" t="inlineStr">
+        <is>
+          <t>prueba</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="20">
+      <c r="A20" s="9">
+        <v>12156</v>
+      </c>
+      <c r="B20" s="9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C20" s="9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D20" s="9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="21">
+      <c r="A21" s="9">
+        <v>92780</v>
+      </c>
+      <c r="B21" s="9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C21" s="9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D21" s="9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -835,80 +1178,79 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.796875" style="10"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>86</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -920,27 +1262,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0852A8F-B607-4A83-B14C-ED5F14713E4C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="56.19921875" customWidth="1"/>
+    <col min="2" max="2" width="56.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="21.75" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -951,7 +1293,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -962,7 +1304,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -973,15 +1315,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -997,14 +1339,14 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -1016,7 +1358,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1030,7 +1372,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1044,7 +1386,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1058,15 +1400,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -1085,22 +1427,22 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.09765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1138,7 +1480,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1176,7 +1518,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1214,7 +1556,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1261,169 +1603,225 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.3984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.796875" style="10"/>
-    <col min="4" max="4" width="16.8984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.796875" style="10"/>
-    <col min="7" max="7" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.296875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="12.59765625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="8.796875" style="10"/>
-    <col min="11" max="11" width="21.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.69921875" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.796875" style="10"/>
+    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.625" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="12" t="s">
+      <c r="I1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="13">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="2" t="s">
         <v>49</v>
       </c>
       <c r="H2" s="3">
         <v>31079</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="2" t="s">
         <v>68</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="13">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="8">
         <v>123456789</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="2" t="s">
         <v>58</v>
       </c>
       <c r="H3" s="3">
         <v>28689</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="2" t="s">
         <v>72</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="14">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E4" s="8">
         <v>987654321</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="2" t="s">
         <v>49</v>
       </c>
       <c r="H4" s="3">
         <v>33918</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="2" t="s">
         <v>77</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="2" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB87FBDE-ED29-4A29-91FF-462EF79043D6}">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
+    <col min="11" max="11" width="17.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
cambios a insertar finalizados
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridia\source\repos\Medical App\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B485BCB-36FB-4E9B-A9AC-01989D2DBCB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AB91E2-1587-4DAC-BB26-E2AC916DC155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
+    <workbookView xWindow="-41388" yWindow="-36" windowWidth="41496" windowHeight="16776" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuarios" sheetId="10" r:id="rId1"/>
+    <sheet name="Usuarios" sheetId="12" r:id="rId1"/>
     <sheet name="Sucursales" sheetId="4" r:id="rId2"/>
     <sheet name="Enfermedades" sheetId="6" r:id="rId3"/>
     <sheet name="Medicamentos" sheetId="8" r:id="rId4"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
   <si>
     <t>Usuario</t>
   </si>
@@ -299,22 +299,7 @@
     <t>guillermo@gmail.com</t>
   </si>
   <si>
-    <t>ss</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>ssss</t>
-  </si>
-  <si>
     <t>Enfermedad</t>
-  </si>
-  <si>
-    <t>dsd</t>
-  </si>
-  <si>
-    <t>sds</t>
   </si>
   <si>
     <t>Medicamentos</t>
@@ -762,15 +747,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{4C3A559B-DF1A-4F29-9E75-ADE6C57A514E}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="false">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -846,16 +834,16 @@
     </row>
     <row outlineLevel="0" r="6">
       <c r="A6" s="9">
-        <v>1</v>
+        <v>90315</v>
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>rrr</t>
+          <t>rdiazelx@gmail.com</t>
         </is>
       </c>
       <c r="C6" s="9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>123</t>
         </is>
       </c>
       <c r="D6" s="9" t="inlineStr">
@@ -864,309 +852,8 @@
         </is>
       </c>
     </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="9">
-        <v>1</v>
-      </c>
-      <c r="B7" s="9" t="inlineStr">
-        <is>
-          <t>rrr</t>
-        </is>
-      </c>
-      <c r="C7" s="9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t>medico</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="8">
-      <c r="A8" s="9">
-        <v>1</v>
-      </c>
-      <c r="B8" s="9" t="inlineStr">
-        <is>
-          <t>rrr</t>
-        </is>
-      </c>
-      <c r="C8" s="9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>medico</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="9">
-      <c r="A9" s="9">
-        <v>1</v>
-      </c>
-      <c r="B9" s="9" t="inlineStr">
-        <is>
-          <t>rrr</t>
-        </is>
-      </c>
-      <c r="C9" s="9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>medico</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="10">
-      <c r="A10" s="9">
-        <v>1</v>
-      </c>
-      <c r="B10" s="9" t="inlineStr">
-        <is>
-          <t>rrr</t>
-        </is>
-      </c>
-      <c r="C10" s="9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>medico</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="11">
-      <c r="A11" s="9">
-        <v>1</v>
-      </c>
-      <c r="B11" s="9" t="inlineStr">
-        <is>
-          <t>rrr</t>
-        </is>
-      </c>
-      <c r="C11" s="9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>medico</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="12">
-      <c r="A12" s="9">
-        <v>1</v>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>rrr</t>
-        </is>
-      </c>
-      <c r="C12" s="9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D12" s="9" t="inlineStr">
-        <is>
-          <t>medico</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="13">
-      <c r="A13" s="9">
-        <v>1</v>
-      </c>
-      <c r="B13" s="9" t="inlineStr">
-        <is>
-          <t>ffaf</t>
-        </is>
-      </c>
-      <c r="C13" s="9" t="inlineStr">
-        <is>
-          <t>fff</t>
-        </is>
-      </c>
-      <c r="D13" s="9" t="inlineStr">
-        <is>
-          <t>fafafa</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="14">
-      <c r="A14" s="9">
-        <v>1</v>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>ffaf</t>
-        </is>
-      </c>
-      <c r="C14" s="9" t="inlineStr">
-        <is>
-          <t>fff</t>
-        </is>
-      </c>
-      <c r="D14" s="9" t="inlineStr">
-        <is>
-          <t>fafafa</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="15">
-      <c r="A15" s="9">
-        <v>41713</v>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>rdiazelx@gmail.com</t>
-        </is>
-      </c>
-      <c r="C15" s="9" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="D15" s="9" t="inlineStr">
-        <is>
-          <t>medico</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="16">
-      <c r="A16" s="9">
-        <v>75928</v>
-      </c>
-      <c r="B16" s="9" t="inlineStr">
-        <is>
-          <t>rttt</t>
-        </is>
-      </c>
-      <c r="C16" s="9" t="inlineStr">
-        <is>
-          <t>tttt</t>
-        </is>
-      </c>
-      <c r="D16" s="9" t="inlineStr">
-        <is>
-          <t>ttt</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="17">
-      <c r="A17" s="9">
-        <v>16425</v>
-      </c>
-      <c r="B17" s="9" t="inlineStr">
-        <is>
-          <t>rdiazelx@gmail.com</t>
-        </is>
-      </c>
-      <c r="C17" s="9" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="D17" s="9" t="inlineStr">
-        <is>
-          <t>administrador</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="18">
-      <c r="A18" s="9">
-        <v>54053</v>
-      </c>
-      <c r="B18" s="9" t="inlineStr">
-        <is>
-          <t>jack</t>
-        </is>
-      </c>
-      <c r="C18" s="9" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="D18" s="9" t="inlineStr">
-        <is>
-          <t>medico</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="19">
-      <c r="A19" s="9">
-        <v>79710</v>
-      </c>
-      <c r="B19" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="C19" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="D19" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="20">
-      <c r="A20" s="9">
-        <v>12156</v>
-      </c>
-      <c r="B20" s="9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C20" s="9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D20" s="9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="21">
-      <c r="A21" s="9">
-        <v>92780</v>
-      </c>
-      <c r="B21" s="9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C21" s="9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="D21" s="9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1175,7 +862,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,18 +927,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>85</v>
-      </c>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1262,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0852A8F-B607-4A83-B14C-ED5F14713E4C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +955,7 @@
         <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
@@ -1316,15 +995,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>90</v>
-      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1336,7 +1008,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,18 +1073,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1424,7 +1086,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1432,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,37 +1446,37 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G1" t="s">
         <v>82</v>
       </c>
       <c r="H1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="J1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="K1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="L1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
finalizado, faltan detalles de limpiar textbox
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridia\source\repos\Medical App\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AB91E2-1587-4DAC-BB26-E2AC916DC155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000A40B8-206F-4FA4-B7D2-CE2441B02D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-41388" yWindow="-36" windowWidth="41496" windowHeight="16776" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuarios" sheetId="12" r:id="rId1"/>
+    <sheet name="Usuarios" sheetId="13" r:id="rId1"/>
     <sheet name="Sucursales" sheetId="4" r:id="rId2"/>
-    <sheet name="Enfermedades" sheetId="6" r:id="rId3"/>
+    <sheet name="Enfermedades" sheetId="14" r:id="rId3"/>
     <sheet name="Medicamentos" sheetId="8" r:id="rId4"/>
     <sheet name="Pacientes" sheetId="7" r:id="rId5"/>
     <sheet name="Medicos" sheetId="9" r:id="rId6"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
   <si>
     <t>Usuario</t>
   </si>
@@ -120,18 +120,6 @@
   </si>
   <si>
     <t>Id</t>
-  </si>
-  <si>
-    <t>Dengue</t>
-  </si>
-  <si>
-    <t>Virus</t>
-  </si>
-  <si>
-    <t>Covid</t>
-  </si>
-  <si>
-    <t>Influenza</t>
   </si>
   <si>
     <t>Farmacéutica</t>
@@ -747,22 +735,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{4C3A559B-DF1A-4F29-9E75-ADE6C57A514E}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF4A275-F396-4E47-A64D-E4BA73D60EA3}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -776,7 +761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -790,26 +775,26 @@
         <v>12</v>
       </c>
     </row>
-    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C3" s="7">
         <v>123</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C4" s="7">
         <v>456</v>
@@ -818,58 +803,18 @@
         <v>12</v>
       </c>
     </row>
-    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C5" s="7">
         <v>456</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="9">
-        <v>90315</v>
-      </c>
-      <c r="B6" s="9" t="inlineStr">
-        <is>
-          <t>rdiazelx@gmail.com</t>
-        </is>
-      </c>
-      <c r="C6" s="9" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="D6" s="9" t="inlineStr">
-        <is>
-          <t>medico</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="9">
-        <v>24912</v>
-      </c>
-      <c r="B7" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="C7" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -882,7 +827,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,7 +846,7 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -958,16 +903,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{C0852A8F-B607-4A83-B14C-ED5F14713E4C}">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{8388D3D7-57A3-4512-A480-B338B3050F66}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="false">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="56.25" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row spans="1:3" ht="21.75" x14ac:dyDescent="0.6" outlineLevel="0" r="1">
@@ -975,211 +920,60 @@
         <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row spans="1:3" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-    </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="9">
-        <v>57273</v>
-      </c>
-      <c r="B6" s="9" t="inlineStr">
+    <row outlineLevel="0" r="2">
+      <c r="A2" s="9" t="inlineStr">
         <is>
-          <t>Fiebre</t>
+          <t>53897</t>
         </is>
       </c>
-      <c r="C6" s="9" t="inlineStr">
+      <c r="B2" s="9" t="inlineStr">
         <is>
-          <t>Aumento de la temperatura corporal por encima de lo normal (98,6 grados F), generalmente causado por una enfermedad.</t>
+          <t>Gripe</t>
         </is>
       </c>
-    </row>
-    <row outlineLevel="0" r="7">
-      <c r="A7" s="9">
-        <v>21574</v>
-      </c>
-      <c r="B7" s="9" t="inlineStr">
+      <c r="C2" s="9" t="inlineStr">
         <is>
-          <t>Dengue</t>
+          <t>Enfermedad viral respiratoria con fiebre, dolor de garganta y dolores musculares.</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>El dengue es una enfermedad viral transmitida por mosquitos y causa fiebre, dolor de cabeza y erupción cutánea.</t>
+          <t>60396</t>
         </is>
       </c>
-    </row>
-    <row outlineLevel="0" r="8">
-      <c r="A8" s="9">
-        <v>31247</v>
-      </c>
-      <c r="B8" s="9" t="inlineStr">
+      <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>Gastritis</t>
+          <t>Covid</t>
         </is>
       </c>
-      <c r="C8" s="9" t="inlineStr">
+      <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>La gastritis es la inflamación del revestimiento del estómago que causa dolor abdominal y otros síntomas.</t>
+          <t> Enfermedad infecciosa causada por el virus SARS-CoV-2, con síntomas como fiebre, tos seca y dificultad para respirar.</t>
         </is>
       </c>
     </row>
-    <row outlineLevel="0" r="9">
-      <c r="A9" s="9">
-        <v>64231</v>
-      </c>
-      <c r="B9" s="9" t="inlineStr">
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>Pulmonia</t>
+          <t>99868</t>
         </is>
       </c>
-      <c r="C9" s="9" t="inlineStr">
+      <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>La pulmonía es una infección en los pulmones que causa síntomas como fiebre, tos, dificultad para respirar y malestar general.</t>
+          <t>Neumonía</t>
         </is>
       </c>
-    </row>
-    <row outlineLevel="0" r="10">
-      <c r="A10" s="9">
-        <v>30645</v>
-      </c>
-      <c r="B10" s="9" t="inlineStr">
+      <c r="C4" s="9" t="inlineStr">
         <is>
-          <t>Migraña</t>
-        </is>
-      </c>
-      <c r="C10" s="9" t="inlineStr">
-        <is>
-          <t>La migraña es un tipo de dolor de cabeza intenso y recurrente, que suele ser pulsátil y puede estar acompañado de náuseas, vómitos y sensibilidad a la luz y al sonido.</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="11">
-      <c r="A11" s="9">
-        <v>39039</v>
-      </c>
-      <c r="B11" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="C11" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="12">
-      <c r="A12" s="9">
-        <v>31779</v>
-      </c>
-      <c r="B12" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="C12" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="13">
-      <c r="A13" s="9">
-        <v>83298</v>
-      </c>
-      <c r="B13" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="C13" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="14">
-      <c r="A14" s="9">
-        <v>75570</v>
-      </c>
-      <c r="B14" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="C14" s="9" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="15">
-      <c r="A15" s="9">
-        <v>14953</v>
-      </c>
-      <c r="B15" s="9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C15" s="9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="16">
-      <c r="A16" s="9">
-        <v>84866</v>
-      </c>
-      <c r="B16" s="9" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
-      <c r="C16" s="9" t="inlineStr">
-        <is>
-          <t>f</t>
+          <t>Infección del tejido pulmonar que causa inflamación y dificultad respiratoria.</t>
         </is>
       </c>
     </row>
@@ -1189,77 +983,96 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F1A546-74ED-4339-A07B-8B9763880824}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{43F1A546-74ED-4339-A07B-8B9763880824}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+    <sheetView workbookViewId="0" rightToLeft="false">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D3" s="2">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D4" s="2">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="9">
+        <v>40168</v>
+      </c>
+      <c r="B6" s="9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D6" s="9">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1297,22 +1110,22 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
@@ -1324,7 +1137,7 @@
         <v>14</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1332,37 +1145,37 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2">
         <v>123456789</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H2" s="3">
         <v>32874</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1370,37 +1183,37 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="H3" s="3">
         <v>31213</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1408,37 +1221,37 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2">
         <v>456789123</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H4" s="3">
         <v>34768</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1474,31 +1287,31 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1506,34 +1319,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H2" s="3">
         <v>31079</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1541,34 +1354,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E3" s="8">
         <v>123456789</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H3" s="3">
         <v>28689</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1576,34 +1389,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E4" s="8">
         <v>987654321</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H4" s="3">
         <v>33918</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1631,37 +1444,37 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s">
         <v>82</v>
       </c>
-      <c r="H1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" t="s">
-        <v>86</v>
-      </c>
       <c r="J1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="K1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
agregado expediente medico. funcionando
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridia\source\repos\Medical App\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000A40B8-206F-4FA4-B7D2-CE2441B02D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F51ADB-DF66-4FA1-BCF1-1B71E1C34783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41388" yWindow="-36" windowWidth="41496" windowHeight="16776" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
+    <workbookView xWindow="-41388" yWindow="-36" windowWidth="41496" windowHeight="16776" activeTab="6" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="13" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="104">
   <si>
     <t>Usuario</t>
   </si>
@@ -308,16 +308,52 @@
     <t>fechaNacimiento</t>
   </si>
   <si>
-    <t>apellido2</t>
-  </si>
-  <si>
-    <t>apellido1</t>
-  </si>
-  <si>
     <t>nombre</t>
   </si>
   <si>
     <t>idPaciente</t>
+  </si>
+  <si>
+    <t>53897</t>
+  </si>
+  <si>
+    <t>Gripe</t>
+  </si>
+  <si>
+    <t>Enfermedad viral respiratoria con fiebre, dolor de garganta y dolores musculares.</t>
+  </si>
+  <si>
+    <t>60396</t>
+  </si>
+  <si>
+    <t>Covid</t>
+  </si>
+  <si>
+    <t>Enfermedad infecciosa causada por el virus SARS-CoV-2, con síntomas como fiebre, tos seca y dificultad para respirar.</t>
+  </si>
+  <si>
+    <t>99868</t>
+  </si>
+  <si>
+    <t>Neumonía</t>
+  </si>
+  <si>
+    <t>Infección del tejido pulmonar que causa inflamación y dificultad respiratoria.</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Gómez A</t>
+  </si>
+  <si>
+    <t>Alejandro González</t>
+  </si>
+  <si>
+    <t>Tomar 1 cada 12 horas</t>
+  </si>
+  <si>
+    <t>apellido</t>
   </si>
 </sst>
 </file>
@@ -373,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -402,6 +438,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,7 +775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF4A275-F396-4E47-A64D-E4BA73D60EA3}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -827,7 +864,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,10 +940,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{8388D3D7-57A3-4512-A480-B338B3050F66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8388D3D7-57A3-4512-A480-B338B3050F66}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="false">
+    <sheetView workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
@@ -915,7 +952,7 @@
     <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:3" ht="21.75" x14ac:dyDescent="0.6" outlineLevel="0" r="1">
+    <row r="1" spans="1:3" ht="21.75" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -926,55 +963,37 @@
         <v>9</v>
       </c>
     </row>
-    <row outlineLevel="0" r="2">
-      <c r="A2" s="9" t="inlineStr">
-        <is>
-          <t>53897</t>
-        </is>
-      </c>
-      <c r="B2" s="9" t="inlineStr">
-        <is>
-          <t>Gripe</t>
-        </is>
-      </c>
-      <c r="C2" s="9" t="inlineStr">
-        <is>
-          <t>Enfermedad viral respiratoria con fiebre, dolor de garganta y dolores musculares.</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="3">
-      <c r="A3" s="9" t="inlineStr">
-        <is>
-          <t>60396</t>
-        </is>
-      </c>
-      <c r="B3" s="9" t="inlineStr">
-        <is>
-          <t>Covid</t>
-        </is>
-      </c>
-      <c r="C3" s="9" t="inlineStr">
-        <is>
-          <t> Enfermedad infecciosa causada por el virus SARS-CoV-2, con síntomas como fiebre, tos seca y dificultad para respirar.</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="4">
-      <c r="A4" s="9" t="inlineStr">
-        <is>
-          <t>99868</t>
-        </is>
-      </c>
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t>Neumonía</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>Infección del tejido pulmonar que causa inflamación y dificultad respiratoria.</t>
-        </is>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -983,11 +1002,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{43F1A546-74ED-4339-A07B-8B9763880824}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F1A546-74ED-4339-A07B-8B9763880824}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="false">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,7 +1015,7 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -1010,7 +1029,7 @@
         <v>27</v>
       </c>
     </row>
-    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1024,7 +1043,7 @@
         <v>100</v>
       </c>
     </row>
-    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1038,7 +1057,7 @@
         <v>200</v>
       </c>
     </row>
-    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1052,23 +1071,19 @@
         <v>150</v>
       </c>
     </row>
-    <row spans="1:4" x14ac:dyDescent="0.25" outlineLevel="0" r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
     </row>
-    <row outlineLevel="0" r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>40168</v>
       </c>
-      <c r="B6" s="9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C6" s="9" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
+      <c r="B6" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="D6" s="9">
         <v>10</v>
@@ -1084,7 +1099,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1279,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,57 +1442,91 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB87FBDE-ED29-4A29-91FF-462EF79043D6}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" customWidth="1"/>
-    <col min="11" max="11" width="17.875" customWidth="1"/>
+    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="H1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3">
+        <v>34768</v>
+      </c>
+      <c r="E2" s="12">
+        <v>45115</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="12">
+        <v>45146</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregada funcion de seleccionar paciente y abrir expediente
</commit_message>
<xml_diff>
--- a/Medical App/Uploads/BaseDeDatos.xlsx
+++ b/Medical App/Uploads/BaseDeDatos.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridia\source\repos\Medical App\Medical App\Uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C792BC87-12A0-48F1-9954-71802BF5994A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCF66A1-B4BE-4153-860B-B25D72678B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41388" yWindow="-36" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{FDFF9493-EB7B-4FF3-896E-D3C23D0B14FF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuarios" sheetId="16" r:id="rId1"/>
-    <sheet name="Sucursales" sheetId="4" r:id="rId2"/>
-    <sheet name="Enfermedades" sheetId="14" r:id="rId3"/>
-    <sheet name="Medicamentos" sheetId="17" r:id="rId4"/>
-    <sheet name="Pacientes" sheetId="7" r:id="rId5"/>
-    <sheet name="Medicos" sheetId="9" r:id="rId6"/>
+    <sheet name="Usuarios" sheetId="23" r:id="rId1"/>
+    <sheet name="Sucursales" sheetId="24" r:id="rId2"/>
+    <sheet name="Enfermedades" sheetId="25" r:id="rId3"/>
+    <sheet name="Medicamentos" sheetId="26" r:id="rId4"/>
+    <sheet name="Pacientes" sheetId="22" r:id="rId5"/>
+    <sheet name="Medicos" sheetId="27" r:id="rId6"/>
     <sheet name="Expedientes" sheetId="15" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
   <si>
     <t>ID</t>
   </si>
@@ -266,6 +266,27 @@
     <t>carlosgomez@example.com</t>
   </si>
   <si>
+    <t>Ricardo</t>
+  </si>
+  <si>
+    <t>Diaz</t>
+  </si>
+  <si>
+    <t>Cédula nacional</t>
+  </si>
+  <si>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>Casado</t>
+  </si>
+  <si>
+    <t>Nacional</t>
+  </si>
+  <si>
+    <t>prueba@prueba.com</t>
+  </si>
+  <si>
     <t>Especialidad</t>
   </si>
   <si>
@@ -335,9 +356,6 @@
     <t>fechaCita</t>
   </si>
   <si>
-    <t>especialidadMedico</t>
-  </si>
-  <si>
     <t>Medicamentos</t>
   </si>
   <si>
@@ -347,20 +365,20 @@
     <t>fechaPrescripcion</t>
   </si>
   <si>
-    <t>Gómez A</t>
-  </si>
-  <si>
     <t>Alejandro González</t>
   </si>
   <si>
     <t>Tomar 1 cada 12 horas</t>
+  </si>
+  <si>
+    <t>especialidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +390,12 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Poppins"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -409,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -438,6 +462,7 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,11 +796,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A4017F-7B61-4940-91C4-B2F97372DC7E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3595CA9C-2433-4FA1-A566-557D909B44D6}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,16 +853,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349371A3-B132-4D64-BA53-AC966C95A385}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2130C34-E37A-478B-898A-EE8A0F97E9E9}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2 A2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -902,20 +927,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8388D3D7-57A3-4512-A480-B338B3050F66}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93E3E461-DA8C-4078-9C86-92FA2230DCD7}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23 F23"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.125" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:3" ht="21.75" x14ac:dyDescent="0.6">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -965,11 +986,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B94C99-6E4E-41F8-83EF-318558B2FE27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55A1489-F0BF-40FA-BEBF-5BD7917155B5}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,27 +1057,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681C15B9-EC30-4BAF-91C3-5E6E8A5EFD20}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02561923-129B-4F52-AD40-308B2777C997}">
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4 H4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -1208,6 +1216,44 @@
       </c>
       <c r="L4" s="2" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>94139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5">
+        <v>111111</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="12">
+        <v>45116</v>
+      </c>
+      <c r="I5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5">
+        <v>50672028241</v>
+      </c>
+      <c r="L5" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1216,27 +1262,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD2C60D-C44E-4300-B74D-8D1941E587B3}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2 I2"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.625" customWidth="1"/>
-    <col min="10" max="10" width="9.5" customWidth="1"/>
-    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.75" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1264,7 +1297,7 @@
         <v>51</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>10</v>
@@ -1278,16 +1311,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>57</v>
@@ -1299,13 +1332,13 @@
         <v>31079</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1313,7 +1346,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>63</v>
@@ -1322,7 +1355,7 @@
         <v>56</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>66</v>
@@ -1334,13 +1367,13 @@
         <v>28689</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1348,16 +1381,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>57</v>
@@ -1369,18 +1402,17 @@
         <v>33918</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1388,74 +1420,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B1396C-C573-4D36-A80D-6055158D332E}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="H1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="I1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="J1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="3">
-        <v>34768</v>
+      <c r="A2">
+        <v>94139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="12">
+        <v>45116</v>
       </c>
       <c r="E2" s="11">
         <v>45115</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="J2" s="11">
         <v>45146</v>

</xml_diff>